<commit_message>
Make Multiple Changes, Add CSS
</commit_message>
<xml_diff>
--- a/hourly_production_lines.xlsx
+++ b/hourly_production_lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OmarPerez/Documents/production_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B2E7A7-4F3C-C247-A5E1-26EC0F66D5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B15A7B7-EA51-2746-A934-B5E7E9284C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1700" windowWidth="27640" windowHeight="16940" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,10 +738,10 @@
         <v>0.25</v>
       </c>
       <c r="B4" s="8">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="C4" s="17">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -750,7 +750,7 @@
         <v>0.25</v>
       </c>
       <c r="G4" s="8">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="H4" s="9">
         <v>230</v>
@@ -791,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="15">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="I5" s="15">
         <v>0</v>
@@ -1043,11 +1043,11 @@
       </c>
       <c r="B12" s="11">
         <f>SUM(B2:B11)</f>
-        <v>321</v>
+        <v>462</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" ref="C12:D12" si="0">SUM(C2:C11)</f>
-        <v>2185</v>
+        <v>2109</v>
       </c>
       <c r="D12" s="12">
         <f t="shared" si="0"/>
@@ -1058,11 +1058,11 @@
       </c>
       <c r="G12" s="11">
         <f>SUM(G2:G11)</f>
-        <v>169</v>
+        <v>326</v>
       </c>
       <c r="H12" s="12">
         <f t="shared" ref="H12:I12" si="1">SUM(H2:H11)</f>
-        <v>2185</v>
+        <v>2109</v>
       </c>
       <c r="I12" s="12">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Implement Getting Excel file numbers into code
</commit_message>
<xml_diff>
--- a/hourly_production_lines.xlsx
+++ b/hourly_production_lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OmarPerez/Documents/production_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174A7FB3-FC28-7646-A97F-76750B9C35AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4ABCAD-532B-D24F-9344-B6B5DAE472D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,7 +890,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B8" s="8">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C8" s="17">
         <v>230</v>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B12" s="11">
         <f>SUM(B2:B11)</f>
-        <v>1163</v>
+        <v>1168</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" ref="C12:D12" si="0">SUM(C2:C11)</f>

</xml_diff>

<commit_message>
Make Changes to match case code block
</commit_message>
<xml_diff>
--- a/hourly_production_lines.xlsx
+++ b/hourly_production_lines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OmarPerez/Documents/production_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4ABCAD-532B-D24F-9344-B6B5DAE472D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F8366D-9D4E-7348-B30B-58F7E6A6A5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +686,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L2" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M2" s="5">
         <v>115</v>
@@ -724,7 +724,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="L3" s="4">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="M3" s="5">
         <v>230</v>
@@ -762,7 +762,7 @@
         <v>0.25</v>
       </c>
       <c r="L4" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="9">
         <v>230</v>
@@ -800,7 +800,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="L5" s="14">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="M5" s="15">
         <v>230</v>
@@ -838,7 +838,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="L6" s="4">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="M6" s="5">
         <v>230</v>
@@ -876,7 +876,7 @@
         <v>0.375</v>
       </c>
       <c r="L7" s="8">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M7" s="5">
         <v>230</v>
@@ -914,7 +914,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="L8" s="8">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="M8" s="9">
         <v>230</v>
@@ -928,7 +928,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="C9" s="17">
         <v>230</v>
@@ -940,7 +940,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="H9" s="15">
         <v>230</v>
@@ -952,7 +952,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="L9" s="8">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="M9" s="15">
         <v>230</v>
@@ -966,7 +966,7 @@
         <v>0.5</v>
       </c>
       <c r="B10" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C10" s="16">
         <v>230</v>
@@ -978,7 +978,7 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="8">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="H10" s="5">
         <v>230</v>
@@ -990,7 +990,7 @@
         <v>0.5</v>
       </c>
       <c r="L10" s="8">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="M10" s="5">
         <v>230</v>
@@ -1004,7 +1004,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="B11" s="8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C11" s="9">
         <v>230</v>
@@ -1016,7 +1016,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="H11" s="9">
         <v>230</v>
@@ -1028,7 +1028,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="L11" s="8">
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="M11" s="9">
         <v>230</v>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B12" s="11">
         <f>SUM(B2:B11)</f>
-        <v>1168</v>
+        <v>1482</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" ref="C12:D12" si="0">SUM(C2:C11)</f>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G12" s="11">
         <f>SUM(G2:G11)</f>
-        <v>908</v>
+        <v>1516</v>
       </c>
       <c r="H12" s="12">
         <f t="shared" ref="H12:I12" si="1">SUM(H2:H11)</f>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="L12" s="11">
         <f>SUM(L2:L11)</f>
-        <v>0</v>
+        <v>1679</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" ref="M12:N12" si="2">SUM(M2:M11)</f>

</xml_diff>

<commit_message>
Make Adjustments Add More Cases
</commit_message>
<xml_diff>
--- a/hourly_production_lines.xlsx
+++ b/hourly_production_lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/OmarPerez/Documents/production_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F8366D-9D4E-7348-B30B-58F7E6A6A5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E62A20-560D-B241-8833-AE3E504965C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{81E560FD-B0FE-C94C-8FE2-30D0BC964491}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,7 +662,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="B2" s="4">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5">
         <v>115</v>
@@ -674,7 +674,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="G2" s="4">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="H2" s="5">
         <v>115</v>
@@ -686,7 +686,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L2" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M2" s="5">
         <v>115</v>
@@ -700,7 +700,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="B3" s="4">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C3" s="16">
         <v>230</v>
@@ -712,7 +712,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="G3" s="4">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="H3" s="5">
         <v>230</v>
@@ -724,7 +724,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="L3" s="4">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="M3" s="5">
         <v>230</v>
@@ -737,9 +737,7 @@
       <c r="A4" s="7">
         <v>0.25</v>
       </c>
-      <c r="B4" s="8">
-        <v>141</v>
-      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="17">
         <v>154</v>
       </c>
@@ -749,9 +747,7 @@
       <c r="F4" s="7">
         <v>0.25</v>
       </c>
-      <c r="G4" s="8">
-        <v>157</v>
-      </c>
+      <c r="G4" s="8"/>
       <c r="H4" s="9">
         <v>230</v>
       </c>
@@ -761,9 +757,7 @@
       <c r="K4" s="7">
         <v>0.25</v>
       </c>
-      <c r="L4" s="8">
-        <v>4</v>
-      </c>
+      <c r="L4" s="8"/>
       <c r="M4" s="9">
         <v>230</v>
       </c>
@@ -775,9 +769,7 @@
       <c r="A5" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="14">
-        <v>223</v>
-      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="17">
         <v>230</v>
       </c>
@@ -787,9 +779,7 @@
       <c r="F5" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="G5" s="14">
-        <v>187</v>
-      </c>
+      <c r="G5" s="14"/>
       <c r="H5" s="15">
         <v>154</v>
       </c>
@@ -799,9 +789,7 @@
       <c r="K5" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="L5" s="14">
-        <v>390</v>
-      </c>
+      <c r="L5" s="14"/>
       <c r="M5" s="15">
         <v>230</v>
       </c>
@@ -813,9 +801,7 @@
       <c r="A6" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B6" s="4">
-        <v>112</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="16">
         <v>230</v>
       </c>
@@ -825,9 +811,7 @@
       <c r="F6" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G6" s="4">
-        <v>152</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="5">
         <v>230</v>
       </c>
@@ -837,9 +821,7 @@
       <c r="K6" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L6" s="4">
-        <v>89</v>
-      </c>
+      <c r="L6" s="4"/>
       <c r="M6" s="5">
         <v>230</v>
       </c>
@@ -851,9 +833,7 @@
       <c r="A7" s="7">
         <v>0.375</v>
       </c>
-      <c r="B7" s="8">
-        <v>155</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="16">
         <v>230</v>
       </c>
@@ -863,9 +843,7 @@
       <c r="F7" s="7">
         <v>0.375</v>
       </c>
-      <c r="G7" s="8">
-        <v>164</v>
-      </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="5">
         <v>230</v>
       </c>
@@ -875,9 +853,7 @@
       <c r="K7" s="7">
         <v>0.375</v>
       </c>
-      <c r="L7" s="8">
-        <v>29</v>
-      </c>
+      <c r="L7" s="8"/>
       <c r="M7" s="5">
         <v>230</v>
       </c>
@@ -889,9 +865,7 @@
       <c r="A8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B8" s="8">
-        <v>216</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="17">
         <v>230</v>
       </c>
@@ -901,9 +875,7 @@
       <c r="F8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G8" s="8">
-        <v>79</v>
-      </c>
+      <c r="G8" s="8"/>
       <c r="H8" s="9">
         <v>230</v>
       </c>
@@ -913,9 +885,7 @@
       <c r="K8" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="L8" s="8">
-        <v>289</v>
-      </c>
+      <c r="L8" s="8"/>
       <c r="M8" s="9">
         <v>230</v>
       </c>
@@ -927,9 +897,7 @@
       <c r="A9" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B9" s="8">
-        <v>114</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="17">
         <v>230</v>
       </c>
@@ -939,9 +907,7 @@
       <c r="F9" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G9" s="8">
-        <v>202</v>
-      </c>
+      <c r="G9" s="8"/>
       <c r="H9" s="15">
         <v>230</v>
       </c>
@@ -951,9 +917,7 @@
       <c r="K9" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L9" s="8">
-        <v>298</v>
-      </c>
+      <c r="L9" s="8"/>
       <c r="M9" s="15">
         <v>230</v>
       </c>
@@ -965,9 +929,7 @@
       <c r="A10" s="7">
         <v>0.5</v>
       </c>
-      <c r="B10" s="8">
-        <v>100</v>
-      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="16">
         <v>230</v>
       </c>
@@ -977,9 +939,7 @@
       <c r="F10" s="7">
         <v>0.5</v>
       </c>
-      <c r="G10" s="8">
-        <v>203</v>
-      </c>
+      <c r="G10" s="8"/>
       <c r="H10" s="5">
         <v>230</v>
       </c>
@@ -989,9 +949,7 @@
       <c r="K10" s="7">
         <v>0.5</v>
       </c>
-      <c r="L10" s="8">
-        <v>38</v>
-      </c>
+      <c r="L10" s="8"/>
       <c r="M10" s="5">
         <v>230</v>
       </c>
@@ -1003,9 +961,7 @@
       <c r="A11" s="7">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B11" s="8">
-        <v>100</v>
-      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="9">
         <v>230</v>
       </c>
@@ -1015,9 +971,7 @@
       <c r="F11" s="7">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G11" s="8">
-        <v>203</v>
-      </c>
+      <c r="G11" s="8"/>
       <c r="H11" s="9">
         <v>230</v>
       </c>
@@ -1027,9 +981,7 @@
       <c r="K11" s="7">
         <v>0.54166666666666663</v>
       </c>
-      <c r="L11" s="8">
-        <v>239</v>
-      </c>
+      <c r="L11" s="8"/>
       <c r="M11" s="9">
         <v>230</v>
       </c>
@@ -1043,7 +995,7 @@
       </c>
       <c r="B12" s="11">
         <f>SUM(B2:B11)</f>
-        <v>1482</v>
+        <v>311</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" ref="C12:D12" si="0">SUM(C2:C11)</f>
@@ -1058,7 +1010,7 @@
       </c>
       <c r="G12" s="11">
         <f>SUM(G2:G11)</f>
-        <v>1516</v>
+        <v>266</v>
       </c>
       <c r="H12" s="12">
         <f t="shared" ref="H12:I12" si="1">SUM(H2:H11)</f>
@@ -1073,7 +1025,7 @@
       </c>
       <c r="L12" s="11">
         <f>SUM(L2:L11)</f>
-        <v>1679</v>
+        <v>192</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" ref="M12:N12" si="2">SUM(M2:M11)</f>

</xml_diff>